<commit_message>
code refactor and model 4
</commit_message>
<xml_diff>
--- a/output/metric/all scores.xlsx
+++ b/output/metric/all scores.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jacop\Desktop\python projects\M5-kaggle\output\metric\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2731332-4F38-463D-9306-B9BA535D35E3}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E278EEE-7252-48F6-986D-EA8302183ABC}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="27">
   <si>
     <t>date and time</t>
   </si>
@@ -97,6 +97,15 @@
   </si>
   <si>
     <t>lgbm3.lags2+simple.sub.csv</t>
+  </si>
+  <si>
+    <t>best</t>
+  </si>
+  <si>
+    <t>best.trn.feather</t>
+  </si>
+  <si>
+    <t>lgbm3.best.sub.csv</t>
   </si>
 </sst>
 </file>
@@ -415,10 +424,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -558,6 +567,32 @@
         <v>23</v>
       </c>
     </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>44140.774085648147</v>
+      </c>
+      <c r="B6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" t="s">
+        <v>25</v>
+      </c>
+      <c r="E6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6">
+        <v>1.92169486412754</v>
+      </c>
+      <c r="G6" t="s">
+        <v>26</v>
+      </c>
+      <c r="H6">
+        <v>0.60338999999999998</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
generate lags try 2
</commit_message>
<xml_diff>
--- a/output/metric/all scores.xlsx
+++ b/output/metric/all scores.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jacop\Desktop\python projects\M5-kaggle\output\metric\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49F94E59-62CC-45F4-8BB8-C93B7E3483A4}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D15A9A8A-6214-473A-80FB-8A76A87B2ADD}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5235" yWindow="5235" windowWidth="17280" windowHeight="8970" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -49,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="32">
   <si>
     <t>date and time</t>
   </si>
@@ -142,6 +143,9 @@
   </si>
   <si>
     <t>lgbm3gap.best.sub.csv</t>
+  </si>
+  <si>
+    <t>validation base with gap to select features</t>
   </si>
 </sst>
 </file>
@@ -476,8 +480,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7:J7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -700,4 +704,32 @@
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E852B035-B45A-4176-9326-512D6BBB4129}">
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="39" customWidth="1"/>
+    <col min="2" max="2" width="13.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1">
+        <v>2.03591244965226</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
changed for training run
</commit_message>
<xml_diff>
--- a/output/metric/all scores.xlsx
+++ b/output/metric/all scores.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jacop\Desktop\python projects\M5-kaggle\output\metric\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D15A9A8A-6214-473A-80FB-8A76A87B2ADD}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66A905F0-A85C-4976-AC0C-DCDCC3EB8A3D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5235" yWindow="5235" windowWidth="17280" windowHeight="8970" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="32">
   <si>
     <t>date and time</t>
   </si>
@@ -708,10 +708,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E852B035-B45A-4176-9326-512D6BBB4129}">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -728,6 +728,14 @@
         <v>2.03591244965226</v>
       </c>
     </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B2">
+        <v>2.02</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>